<commit_message>
Add list sheet example
</commit_message>
<xml_diff>
--- a/godot-luban-data/Configs/Data/__tables__.xlsx
+++ b/godot-luban-data/Configs/Data/__tables__.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23003" windowHeight="11351"/>
+    <workbookView windowWidth="23651" windowHeight="11748"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>##var</t>
   </si>
@@ -224,6 +224,51 @@
   </si>
   <si>
     <t>one</t>
+  </si>
+  <si>
+    <t>Examples.TbExampleList</t>
+  </si>
+  <si>
+    <t>ExampleList</t>
+  </si>
+  <si>
+    <t>../列表表@_示例.xlsx</t>
+  </si>
+  <si>
+    <t>Game.TbCharacterConfig</t>
+  </si>
+  <si>
+    <t>CharacterConfig</t>
+  </si>
+  <si>
+    <t>../J-角色.xlsx</t>
+  </si>
+  <si>
+    <t>Game.TbPlayerInitialConfig</t>
+  </si>
+  <si>
+    <t>PlayerInitialConfig</t>
+  </si>
+  <si>
+    <t>../W-玩家初始化.xlsx</t>
+  </si>
+  <si>
+    <t>Game.TbMainLevelConfig</t>
+  </si>
+  <si>
+    <t>MainLevelConfig</t>
+  </si>
+  <si>
+    <t>../Z-主线关卡.xlsx</t>
+  </si>
+  <si>
+    <t>Game.TbGlobalConfig</t>
+  </si>
+  <si>
+    <t>GlobalConfig</t>
+  </si>
+  <si>
+    <t>../T-通用全局.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1203,13 +1248,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="29.3333333333333" style="2" customWidth="1"/>
@@ -1381,6 +1426,124 @@
         <v>41</v>
       </c>
     </row>
+    <row r="7" customFormat="1" spans="1:10">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" customFormat="1" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" customFormat="1" spans="1:10">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" customFormat="1" spans="1:10">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" customFormat="1" spans="1:10">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" customFormat="1" spans="1:10">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>